<commit_message>
Deployed page one version one of the app. Fixed an issue with game 3 of Smash Data.
</commit_message>
<xml_diff>
--- a/SSBU Code.xlsx
+++ b/SSBU Code.xlsx
@@ -1,23 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\SSBU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riese\Desktop\SmashBros\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD88D2CD-B103-4146-A198-CEC0D9712120}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51600" windowHeight="17700"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SSBU Code" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -131,10 +138,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -276,12 +283,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -291,8 +300,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -573,94 +580,94 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6:P6"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.5703125" customWidth="1"/>
+    <col min="8" max="8" width="23.5546875" customWidth="1"/>
     <col min="9" max="9" width="5" customWidth="1"/>
-    <col min="10" max="10" width="5.28515625" customWidth="1"/>
+    <col min="10" max="10" width="5.33203125" customWidth="1"/>
     <col min="11" max="11" width="7" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" customWidth="1"/>
-    <col min="13" max="13" width="15.7109375" customWidth="1"/>
-    <col min="14" max="14" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" customWidth="1"/>
+    <col min="13" max="13" width="15.6640625" customWidth="1"/>
+    <col min="14" max="14" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="7" customWidth="1"/>
-    <col min="16" max="16" width="15.85546875" customWidth="1"/>
+    <col min="16" max="16" width="15.88671875" customWidth="1"/>
     <col min="17" max="18" width="36" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="3.6640625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="10" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="7" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="8" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="45.85546875" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="65" max="66" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="3.44140625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="45.88671875" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="65" max="66" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -702,7 +709,7 @@
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -743,7 +750,7 @@
         <v>392.625</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -784,7 +791,7 @@
         <v>402.14285714285717</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -825,7 +832,7 @@
         <v>244.61538461538461</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2</v>
       </c>
@@ -851,7 +858,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
@@ -865,7 +872,7 @@
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -876,18 +883,18 @@
       <c r="H6">
         <v>212</v>
       </c>
-      <c r="J6" s="14" t="s">
+      <c r="J6" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="K6" s="15"/>
-      <c r="L6" s="16"/>
-      <c r="N6" s="14" t="s">
+      <c r="K6" s="17"/>
+      <c r="L6" s="18"/>
+      <c r="N6" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="O6" s="15"/>
-      <c r="P6" s="16"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="O6" s="17"/>
+      <c r="P6" s="18"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>3</v>
       </c>
@@ -901,7 +908,7 @@
         <v>3</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -919,7 +926,7 @@
         <f>INDEX($A$2:$H$37,MATCH(LARGE($H$2:$H$37,1),$H$2:$H$37,0),3)</f>
         <v>Matt</v>
       </c>
-      <c r="L7" s="17">
+      <c r="L7" s="14">
         <f>INDEX($A$2:$H$37,MATCH(LARGE($H$2:$H$37,1),$H$2:$H$37,0),8)</f>
         <v>525</v>
       </c>
@@ -930,12 +937,12 @@
         <f>INDEX($A$2:$H$37,MATCH(SMALL($H$2:$H$37,1),$H$2:$H$37,0),3)</f>
         <v>Mikael</v>
       </c>
-      <c r="P7" s="17">
+      <c r="P7" s="14">
         <f>INDEX($A$2:$H$37,MATCH(SMALL($H$2:$H$37,1),$H$2:$H$37,0),8)</f>
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>4</v>
       </c>
@@ -967,7 +974,7 @@
         <f>INDEX($A$2:$H$37,MATCH(LARGE($H$2:$H$37,2),$H$2:$H$37,0),3)</f>
         <v>Robert</v>
       </c>
-      <c r="L8" s="17">
+      <c r="L8" s="14">
         <f>INDEX($A$2:$H$37,MATCH(LARGE($H$2:$H$37,2),$H$2:$H$37,0),8)</f>
         <v>499</v>
       </c>
@@ -978,12 +985,12 @@
         <f>INDEX($A$2:$H$37,MATCH(SMALL($H$2:$H$37,2),$H$2:$H$37,0),3)</f>
         <v>Mikael</v>
       </c>
-      <c r="P8" s="17">
+      <c r="P8" s="14">
         <f>INDEX($A$2:$H$37,MATCH(SMALL($H$2:$H$37,2),$H$2:$H$37,0),8)</f>
         <v>134</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>4</v>
       </c>
@@ -1015,7 +1022,7 @@
         <f>INDEX($A$2:$H$37,MATCH(LARGE($H$2:$H$37,3),$H$2:$H$37,0),3)</f>
         <v>Matt</v>
       </c>
-      <c r="L9" s="18">
+      <c r="L9" s="15">
         <f>INDEX($A$2:$H$37,MATCH(LARGE($H$2:$H$37,3),$H$2:$H$37,0),8)</f>
         <v>485</v>
       </c>
@@ -1026,12 +1033,12 @@
         <f>INDEX($A$2:$H$37,MATCH(SMALL($H$2:$H$37,3),$H$2:$H$37,0),3)</f>
         <v>Mikael</v>
       </c>
-      <c r="P9" s="18">
+      <c r="P9" s="15">
         <f>INDEX($A$2:$H$37,MATCH(SMALL($H$2:$H$37,3),$H$2:$H$37,0),8)</f>
         <v>146</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>5</v>
       </c>
@@ -1057,7 +1064,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>5</v>
       </c>
@@ -1083,7 +1090,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>6</v>
       </c>
@@ -1109,7 +1116,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>6</v>
       </c>
@@ -1135,7 +1142,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>7</v>
       </c>
@@ -1161,7 +1168,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>7</v>
       </c>
@@ -1187,7 +1194,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>8</v>
       </c>
@@ -1213,7 +1220,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>8</v>
       </c>
@@ -1239,7 +1246,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>9</v>
       </c>
@@ -1265,7 +1272,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>9</v>
       </c>
@@ -1291,7 +1298,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>10</v>
       </c>
@@ -1317,7 +1324,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>10</v>
       </c>
@@ -1343,7 +1350,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>11</v>
       </c>
@@ -1369,7 +1376,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>11</v>
       </c>
@@ -1395,7 +1402,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>12</v>
       </c>
@@ -1421,7 +1428,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>12</v>
       </c>
@@ -1447,7 +1454,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>13</v>
       </c>
@@ -1473,7 +1480,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>13</v>
       </c>
@@ -1499,7 +1506,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>14</v>
       </c>
@@ -1525,7 +1532,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>14</v>
       </c>
@@ -1551,7 +1558,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>15</v>
       </c>
@@ -1577,7 +1584,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>15</v>
       </c>
@@ -1603,7 +1610,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>16</v>
       </c>
@@ -1629,7 +1636,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>16</v>
       </c>
@@ -1655,7 +1662,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>17</v>
       </c>
@@ -1681,7 +1688,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>17</v>
       </c>
@@ -1707,7 +1714,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>18</v>
       </c>
@@ -1733,7 +1740,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
Updated the data with September 13th information.
</commit_message>
<xml_diff>
--- a/SSBU Code.xlsx
+++ b/SSBU Code.xlsx
@@ -1,37 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riese\Desktop\SmashBros\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\sancfs001\actuarial$\Staff\Matthew Jones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD88D2CD-B103-4146-A198-CEC0D9712120}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51600" windowHeight="17700"/>
   </bookViews>
   <sheets>
     <sheet name="SSBU Code" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="31">
   <si>
     <t>Matt</t>
   </si>
@@ -117,33 +110,20 @@
     <t>Fox</t>
   </si>
   <si>
-    <t xml:space="preserve">Max Given </t>
-  </si>
-  <si>
-    <t>Min Given</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Average Damage </t>
-  </si>
-  <si>
-    <t>Wins</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Win Percentage </t>
-  </si>
-  <si>
-    <t>Names</t>
+    <t>LittleMac</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matt </t>
+  </si>
+  <si>
+    <t>Bayonetta</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="165" formatCode="0.0%"/>
-  </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,29 +139,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -189,121 +156,17 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -580,94 +443,94 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.5546875" customWidth="1"/>
+    <col min="8" max="8" width="23.5703125" customWidth="1"/>
     <col min="9" max="9" width="5" customWidth="1"/>
-    <col min="10" max="10" width="5.33203125" customWidth="1"/>
+    <col min="10" max="10" width="5.28515625" customWidth="1"/>
     <col min="11" max="11" width="7" customWidth="1"/>
-    <col min="12" max="12" width="10.6640625" customWidth="1"/>
-    <col min="13" max="13" width="15.6640625" customWidth="1"/>
-    <col min="14" max="14" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" customWidth="1"/>
+    <col min="14" max="14" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="7" customWidth="1"/>
-    <col min="16" max="16" width="15.88671875" customWidth="1"/>
+    <col min="16" max="16" width="15.85546875" customWidth="1"/>
     <col min="17" max="18" width="36" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="4.109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="3.7109375" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="10" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="7" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="8" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="4.44140625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="4.5546875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="45.88671875" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="26.44140625" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="65" max="66" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="45.85546875" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="65" max="66" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -692,24 +555,10 @@
       <c r="H1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -734,23 +583,8 @@
       <c r="H2">
         <v>480</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="L2" s="7">
-        <f>SUMIF($C$2:$C$37,K2,$F$2:$F$37)</f>
-        <v>11</v>
-      </c>
-      <c r="M2" s="8">
-        <f>L2/COUNTIF($C$2:$C$37,K2)</f>
-        <v>0.6875</v>
-      </c>
-      <c r="N2" s="9">
-        <f>AVERAGEIF($C$2:$C$37,K2,$H$2:$H$37)</f>
-        <v>392.625</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -775,23 +609,8 @@
       <c r="H3">
         <v>412</v>
       </c>
-      <c r="K3" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="L3" s="7">
-        <f t="shared" ref="L3" si="0">SUMIF($C$2:$C$37,K3,$F$2:$F$37)</f>
-        <v>5</v>
-      </c>
-      <c r="M3" s="8">
-        <f t="shared" ref="M3:M4" si="1">L3/COUNTIF($C$2:$C$37,K3)</f>
-        <v>0.7142857142857143</v>
-      </c>
-      <c r="N3" s="9">
-        <f t="shared" ref="N3:N4" si="2">AVERAGEIF($C$2:$C$37,K3,$H$2:$H$37)</f>
-        <v>402.14285714285717</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -816,23 +635,8 @@
       <c r="H4">
         <v>392</v>
       </c>
-      <c r="K4" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="L4" s="11">
-        <f>SUMIF($C$2:$C$37,K4,$F$2:$F$37)</f>
-        <v>2</v>
-      </c>
-      <c r="M4" s="12">
-        <f t="shared" si="1"/>
-        <v>0.15384615384615385</v>
-      </c>
-      <c r="N4" s="13">
-        <f t="shared" si="2"/>
-        <v>244.61538461538461</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -858,7 +662,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -883,18 +687,8 @@
       <c r="H6">
         <v>212</v>
       </c>
-      <c r="J6" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="K6" s="17"/>
-      <c r="L6" s="18"/>
-      <c r="N6" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="O6" s="17"/>
-      <c r="P6" s="18"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -919,30 +713,8 @@
       <c r="H7">
         <v>273</v>
       </c>
-      <c r="J7" s="6">
-        <v>1</v>
-      </c>
-      <c r="K7" s="7" t="str">
-        <f>INDEX($A$2:$H$37,MATCH(LARGE($H$2:$H$37,1),$H$2:$H$37,0),3)</f>
-        <v>Matt</v>
-      </c>
-      <c r="L7" s="14">
-        <f>INDEX($A$2:$H$37,MATCH(LARGE($H$2:$H$37,1),$H$2:$H$37,0),8)</f>
-        <v>525</v>
-      </c>
-      <c r="N7" s="6">
-        <v>1</v>
-      </c>
-      <c r="O7" s="7" t="str">
-        <f>INDEX($A$2:$H$37,MATCH(SMALL($H$2:$H$37,1),$H$2:$H$37,0),3)</f>
-        <v>Mikael</v>
-      </c>
-      <c r="P7" s="14">
-        <f>INDEX($A$2:$H$37,MATCH(SMALL($H$2:$H$37,1),$H$2:$H$37,0),8)</f>
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -967,30 +739,8 @@
       <c r="H8">
         <v>295</v>
       </c>
-      <c r="J8" s="6">
-        <v>2</v>
-      </c>
-      <c r="K8" s="7" t="str">
-        <f>INDEX($A$2:$H$37,MATCH(LARGE($H$2:$H$37,2),$H$2:$H$37,0),3)</f>
-        <v>Robert</v>
-      </c>
-      <c r="L8" s="14">
-        <f>INDEX($A$2:$H$37,MATCH(LARGE($H$2:$H$37,2),$H$2:$H$37,0),8)</f>
-        <v>499</v>
-      </c>
-      <c r="N8" s="6">
-        <v>2</v>
-      </c>
-      <c r="O8" s="7" t="str">
-        <f>INDEX($A$2:$H$37,MATCH(SMALL($H$2:$H$37,2),$H$2:$H$37,0),3)</f>
-        <v>Mikael</v>
-      </c>
-      <c r="P8" s="14">
-        <f>INDEX($A$2:$H$37,MATCH(SMALL($H$2:$H$37,2),$H$2:$H$37,0),8)</f>
-        <v>134</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4</v>
       </c>
@@ -1015,30 +765,8 @@
       <c r="H9">
         <v>439</v>
       </c>
-      <c r="J9" s="10">
-        <v>3</v>
-      </c>
-      <c r="K9" s="11" t="str">
-        <f>INDEX($A$2:$H$37,MATCH(LARGE($H$2:$H$37,3),$H$2:$H$37,0),3)</f>
-        <v>Matt</v>
-      </c>
-      <c r="L9" s="15">
-        <f>INDEX($A$2:$H$37,MATCH(LARGE($H$2:$H$37,3),$H$2:$H$37,0),8)</f>
-        <v>485</v>
-      </c>
-      <c r="N9" s="10">
-        <v>3</v>
-      </c>
-      <c r="O9" s="11" t="str">
-        <f>INDEX($A$2:$H$37,MATCH(SMALL($H$2:$H$37,3),$H$2:$H$37,0),3)</f>
-        <v>Mikael</v>
-      </c>
-      <c r="P9" s="15">
-        <f>INDEX($A$2:$H$37,MATCH(SMALL($H$2:$H$37,3),$H$2:$H$37,0),8)</f>
-        <v>146</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5</v>
       </c>
@@ -1064,7 +792,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>5</v>
       </c>
@@ -1090,7 +818,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>6</v>
       </c>
@@ -1116,7 +844,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>6</v>
       </c>
@@ -1142,7 +870,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>7</v>
       </c>
@@ -1168,7 +896,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>7</v>
       </c>
@@ -1194,7 +922,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>8</v>
       </c>
@@ -1220,7 +948,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>8</v>
       </c>
@@ -1246,7 +974,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>9</v>
       </c>
@@ -1272,7 +1000,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>9</v>
       </c>
@@ -1298,7 +1026,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>10</v>
       </c>
@@ -1324,7 +1052,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>10</v>
       </c>
@@ -1350,7 +1078,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>11</v>
       </c>
@@ -1376,7 +1104,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>11</v>
       </c>
@@ -1402,7 +1130,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>12</v>
       </c>
@@ -1428,7 +1156,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>12</v>
       </c>
@@ -1454,7 +1182,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>13</v>
       </c>
@@ -1480,7 +1208,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>13</v>
       </c>
@@ -1506,7 +1234,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>14</v>
       </c>
@@ -1532,7 +1260,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>14</v>
       </c>
@@ -1558,7 +1286,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>15</v>
       </c>
@@ -1584,7 +1312,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>15</v>
       </c>
@@ -1610,7 +1338,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>16</v>
       </c>
@@ -1636,7 +1364,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>16</v>
       </c>
@@ -1662,7 +1390,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>17</v>
       </c>
@@ -1688,7 +1416,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>17</v>
       </c>
@@ -1714,7 +1442,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>18</v>
       </c>
@@ -1740,7 +1468,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>18</v>
       </c>
@@ -1766,11 +1494,683 @@
         <v>499</v>
       </c>
     </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>19</v>
+      </c>
+      <c r="B38" s="1">
+        <v>43721</v>
+      </c>
+      <c r="C38" t="s">
+        <v>2</v>
+      </c>
+      <c r="D38" t="s">
+        <v>3</v>
+      </c>
+      <c r="E38" t="s">
+        <v>27</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+      <c r="G38">
+        <v>3</v>
+      </c>
+      <c r="H38">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>19</v>
+      </c>
+      <c r="B39" s="1">
+        <v>43721</v>
+      </c>
+      <c r="C39" t="s">
+        <v>3</v>
+      </c>
+      <c r="D39" t="s">
+        <v>2</v>
+      </c>
+      <c r="E39" t="s">
+        <v>11</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>2</v>
+      </c>
+      <c r="H39">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>20</v>
+      </c>
+      <c r="B40" s="1">
+        <v>43721</v>
+      </c>
+      <c r="C40" t="s">
+        <v>2</v>
+      </c>
+      <c r="D40" t="s">
+        <v>0</v>
+      </c>
+      <c r="E40" t="s">
+        <v>27</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+      <c r="G40">
+        <v>3</v>
+      </c>
+      <c r="H40">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>20</v>
+      </c>
+      <c r="B41" s="1">
+        <v>43721</v>
+      </c>
+      <c r="C41" t="s">
+        <v>0</v>
+      </c>
+      <c r="D41" t="s">
+        <v>2</v>
+      </c>
+      <c r="E41" t="s">
+        <v>28</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>2</v>
+      </c>
+      <c r="H41">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>21</v>
+      </c>
+      <c r="B42" s="1">
+        <v>43721</v>
+      </c>
+      <c r="C42" t="s">
+        <v>2</v>
+      </c>
+      <c r="D42" t="s">
+        <v>3</v>
+      </c>
+      <c r="E42" t="s">
+        <v>27</v>
+      </c>
+      <c r="F42">
+        <v>1</v>
+      </c>
+      <c r="G42">
+        <v>3</v>
+      </c>
+      <c r="H42">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>21</v>
+      </c>
+      <c r="B43" s="1">
+        <v>43721</v>
+      </c>
+      <c r="C43" t="s">
+        <v>3</v>
+      </c>
+      <c r="D43" t="s">
+        <v>2</v>
+      </c>
+      <c r="E43" t="s">
+        <v>13</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>22</v>
+      </c>
+      <c r="B44" s="1">
+        <v>43721</v>
+      </c>
+      <c r="C44" t="s">
+        <v>2</v>
+      </c>
+      <c r="D44" t="s">
+        <v>0</v>
+      </c>
+      <c r="E44" t="s">
+        <v>27</v>
+      </c>
+      <c r="F44">
+        <v>1</v>
+      </c>
+      <c r="G44">
+        <v>3</v>
+      </c>
+      <c r="H44">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>22</v>
+      </c>
+      <c r="B45" s="1">
+        <v>43721</v>
+      </c>
+      <c r="C45" t="s">
+        <v>0</v>
+      </c>
+      <c r="D45" t="s">
+        <v>2</v>
+      </c>
+      <c r="E45" t="s">
+        <v>12</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>23</v>
+      </c>
+      <c r="B46" s="1">
+        <v>43721</v>
+      </c>
+      <c r="C46" t="s">
+        <v>2</v>
+      </c>
+      <c r="D46" t="s">
+        <v>3</v>
+      </c>
+      <c r="E46" t="s">
+        <v>27</v>
+      </c>
+      <c r="F46">
+        <v>1</v>
+      </c>
+      <c r="G46">
+        <v>3</v>
+      </c>
+      <c r="H46">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>23</v>
+      </c>
+      <c r="B47" s="1">
+        <v>43721</v>
+      </c>
+      <c r="C47" t="s">
+        <v>3</v>
+      </c>
+      <c r="D47" t="s">
+        <v>2</v>
+      </c>
+      <c r="E47" t="s">
+        <v>11</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>1</v>
+      </c>
+      <c r="H47">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>24</v>
+      </c>
+      <c r="B48" s="1">
+        <v>43721</v>
+      </c>
+      <c r="C48" t="s">
+        <v>2</v>
+      </c>
+      <c r="D48" t="s">
+        <v>0</v>
+      </c>
+      <c r="E48" t="s">
+        <v>27</v>
+      </c>
+      <c r="F48">
+        <v>1</v>
+      </c>
+      <c r="G48">
+        <v>3</v>
+      </c>
+      <c r="H48">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>24</v>
+      </c>
+      <c r="B49" s="1">
+        <v>43721</v>
+      </c>
+      <c r="C49" t="s">
+        <v>29</v>
+      </c>
+      <c r="D49" t="s">
+        <v>2</v>
+      </c>
+      <c r="E49" t="s">
+        <v>28</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>1</v>
+      </c>
+      <c r="H49">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>25</v>
+      </c>
+      <c r="B50" s="1">
+        <v>43721</v>
+      </c>
+      <c r="C50" t="s">
+        <v>2</v>
+      </c>
+      <c r="D50" t="s">
+        <v>3</v>
+      </c>
+      <c r="E50" t="s">
+        <v>27</v>
+      </c>
+      <c r="F50">
+        <v>1</v>
+      </c>
+      <c r="G50">
+        <v>3</v>
+      </c>
+      <c r="H50">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>25</v>
+      </c>
+      <c r="B51" s="1">
+        <v>43721</v>
+      </c>
+      <c r="C51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D51" t="s">
+        <v>2</v>
+      </c>
+      <c r="E51" t="s">
+        <v>11</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <v>2</v>
+      </c>
+      <c r="H51">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>26</v>
+      </c>
+      <c r="B52" s="1">
+        <v>43721</v>
+      </c>
+      <c r="C52" t="s">
+        <v>2</v>
+      </c>
+      <c r="D52" t="s">
+        <v>0</v>
+      </c>
+      <c r="E52" t="s">
+        <v>27</v>
+      </c>
+      <c r="F52">
+        <v>1</v>
+      </c>
+      <c r="G52">
+        <v>3</v>
+      </c>
+      <c r="H52">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>26</v>
+      </c>
+      <c r="B53" s="1">
+        <v>43721</v>
+      </c>
+      <c r="C53" t="s">
+        <v>0</v>
+      </c>
+      <c r="D53" t="s">
+        <v>2</v>
+      </c>
+      <c r="E53" t="s">
+        <v>28</v>
+      </c>
+      <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <v>1</v>
+      </c>
+      <c r="H53">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>27</v>
+      </c>
+      <c r="B54" s="1">
+        <v>43721</v>
+      </c>
+      <c r="C54" t="s">
+        <v>2</v>
+      </c>
+      <c r="D54" t="s">
+        <v>3</v>
+      </c>
+      <c r="E54" t="s">
+        <v>27</v>
+      </c>
+      <c r="F54">
+        <v>0</v>
+      </c>
+      <c r="G54">
+        <v>2</v>
+      </c>
+      <c r="H54">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>27</v>
+      </c>
+      <c r="B55" s="1">
+        <v>43721</v>
+      </c>
+      <c r="C55" t="s">
+        <v>3</v>
+      </c>
+      <c r="D55" t="s">
+        <v>2</v>
+      </c>
+      <c r="E55" t="s">
+        <v>11</v>
+      </c>
+      <c r="F55">
+        <v>1</v>
+      </c>
+      <c r="G55">
+        <v>3</v>
+      </c>
+      <c r="H55">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>30</v>
+      </c>
+      <c r="B56" s="1">
+        <v>43721</v>
+      </c>
+      <c r="C56" t="s">
+        <v>3</v>
+      </c>
+      <c r="D56" t="s">
+        <v>0</v>
+      </c>
+      <c r="E56" t="s">
+        <v>11</v>
+      </c>
+      <c r="F56">
+        <v>0</v>
+      </c>
+      <c r="G56">
+        <v>1</v>
+      </c>
+      <c r="H56">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>30</v>
+      </c>
+      <c r="B57" s="1">
+        <v>43721</v>
+      </c>
+      <c r="C57" t="s">
+        <v>0</v>
+      </c>
+      <c r="D57" t="s">
+        <v>3</v>
+      </c>
+      <c r="E57" t="s">
+        <v>15</v>
+      </c>
+      <c r="F57">
+        <v>1</v>
+      </c>
+      <c r="G57">
+        <v>3</v>
+      </c>
+      <c r="H57">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>31</v>
+      </c>
+      <c r="B58" s="1">
+        <v>43721</v>
+      </c>
+      <c r="C58" t="s">
+        <v>2</v>
+      </c>
+      <c r="D58" t="s">
+        <v>0</v>
+      </c>
+      <c r="E58" t="s">
+        <v>27</v>
+      </c>
+      <c r="F58">
+        <v>1</v>
+      </c>
+      <c r="G58">
+        <v>3</v>
+      </c>
+      <c r="H58">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>31</v>
+      </c>
+      <c r="B59" s="1">
+        <v>43721</v>
+      </c>
+      <c r="C59" t="s">
+        <v>0</v>
+      </c>
+      <c r="D59" t="s">
+        <v>2</v>
+      </c>
+      <c r="E59" t="s">
+        <v>15</v>
+      </c>
+      <c r="F59">
+        <v>0</v>
+      </c>
+      <c r="G59">
+        <v>1</v>
+      </c>
+      <c r="H59">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>32</v>
+      </c>
+      <c r="B60" s="1">
+        <v>43721</v>
+      </c>
+      <c r="C60" t="s">
+        <v>2</v>
+      </c>
+      <c r="D60" t="s">
+        <v>0</v>
+      </c>
+      <c r="E60" t="s">
+        <v>27</v>
+      </c>
+      <c r="F60">
+        <v>1</v>
+      </c>
+      <c r="G60">
+        <v>3</v>
+      </c>
+      <c r="H60">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>32</v>
+      </c>
+      <c r="B61" s="1">
+        <v>43721</v>
+      </c>
+      <c r="C61" t="s">
+        <v>0</v>
+      </c>
+      <c r="D61" t="s">
+        <v>2</v>
+      </c>
+      <c r="E61" t="s">
+        <v>19</v>
+      </c>
+      <c r="F61">
+        <v>0</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+      <c r="H61">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>33</v>
+      </c>
+      <c r="B62" s="1">
+        <v>43721</v>
+      </c>
+      <c r="C62" t="s">
+        <v>2</v>
+      </c>
+      <c r="D62" t="s">
+        <v>0</v>
+      </c>
+      <c r="E62" t="s">
+        <v>27</v>
+      </c>
+      <c r="F62">
+        <v>1</v>
+      </c>
+      <c r="G62">
+        <v>3</v>
+      </c>
+      <c r="H62">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>33</v>
+      </c>
+      <c r="B63" s="1">
+        <v>43721</v>
+      </c>
+      <c r="C63" t="s">
+        <v>0</v>
+      </c>
+      <c r="D63" t="s">
+        <v>2</v>
+      </c>
+      <c r="E63" t="s">
+        <v>30</v>
+      </c>
+      <c r="F63">
+        <v>0</v>
+      </c>
+      <c r="G63">
+        <v>1</v>
+      </c>
+      <c r="H63">
+        <v>76</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="N6:P6"/>
-    <mergeCell ref="J6:L6"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated with latest data.
</commit_message>
<xml_diff>
--- a/SSBU Code.xlsx
+++ b/SSBU Code.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\sancfs001\actuarial$\Staff\Matthew Jones\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rriesenb\Personal\SmashBros\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="48">
   <si>
     <t>Matt</t>
   </si>
@@ -117,6 +117,57 @@
   </si>
   <si>
     <t>Game</t>
+  </si>
+  <si>
+    <t>Chris</t>
+  </si>
+  <si>
+    <t>ZSS</t>
+  </si>
+  <si>
+    <t>Marcus</t>
+  </si>
+  <si>
+    <t>Samus</t>
+  </si>
+  <si>
+    <t>DiddyKong</t>
+  </si>
+  <si>
+    <t>Ganondorf</t>
+  </si>
+  <si>
+    <t>Luigi</t>
+  </si>
+  <si>
+    <t>Mario</t>
+  </si>
+  <si>
+    <t>Bowser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kirby </t>
+  </si>
+  <si>
+    <t>Lucina</t>
+  </si>
+  <si>
+    <t>DonkeyKong</t>
+  </si>
+  <si>
+    <t>Pichu</t>
+  </si>
+  <si>
+    <t>Pikachu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peach </t>
+  </si>
+  <si>
+    <t>ToonLink</t>
+  </si>
+  <si>
+    <t>Geninja</t>
   </si>
 </sst>
 </file>
@@ -460,16 +511,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K105"/>
+  <dimension ref="A1:K187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="H69" sqref="H69"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.7109375" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="8.7109375" style="4" customWidth="1"/>
@@ -594,12 +645,10 @@
       <c r="K2" s="3"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <f ca="1">IF(ISEVEN( CELL("row",A3)) = TRUE, A2 + 1, A2)</f>
-        <v>1</v>
-      </c>
-      <c r="B3" s="1">
-        <f>B2</f>
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5">
         <v>43707</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -620,12 +669,10 @@
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <f t="shared" ref="A4:A67" ca="1" si="0">IF(ISEVEN( CELL("row",A4)) = TRUE, A3 + 1, A3)</f>
-        <v>2</v>
-      </c>
-      <c r="B4" s="1">
-        <f t="shared" ref="B4:B67" si="1">B3</f>
+      <c r="A4" s="4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5">
         <v>43707</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -646,12 +693,10 @@
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="B5" s="1">
-        <f t="shared" si="1"/>
+      <c r="A5" s="4">
+        <v>2</v>
+      </c>
+      <c r="B5" s="5">
         <v>43707</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -672,12 +717,10 @@
       <c r="K5" s="3"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="B6" s="1">
-        <f t="shared" si="1"/>
+      <c r="A6" s="4">
+        <v>3</v>
+      </c>
+      <c r="B6" s="5">
         <v>43707</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -698,12 +741,10 @@
       <c r="K6" s="3"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="B7" s="1">
-        <f t="shared" si="1"/>
+      <c r="A7" s="4">
+        <v>3</v>
+      </c>
+      <c r="B7" s="5">
         <v>43707</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -724,12 +765,10 @@
       <c r="K7" s="3"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A8" s="4">
         <v>4</v>
       </c>
-      <c r="B8" s="1">
-        <f t="shared" si="1"/>
+      <c r="B8" s="5">
         <v>43707</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -750,12 +789,10 @@
       <c r="K8" s="3"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A9" s="4">
         <v>4</v>
       </c>
-      <c r="B9" s="1">
-        <f t="shared" si="1"/>
+      <c r="B9" s="5">
         <v>43707</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -776,12 +813,10 @@
       <c r="K9" s="3"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A10" s="4">
         <v>5</v>
       </c>
-      <c r="B10" s="1">
-        <f t="shared" si="1"/>
+      <c r="B10" s="5">
         <v>43707</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -802,12 +837,10 @@
       <c r="K10" s="3"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A11" s="4">
         <v>5</v>
       </c>
-      <c r="B11" s="1">
-        <f t="shared" si="1"/>
+      <c r="B11" s="5">
         <v>43707</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -828,12 +861,10 @@
       <c r="K11" s="3"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A12" s="4">
         <v>6</v>
       </c>
-      <c r="B12" s="1">
-        <f t="shared" si="1"/>
+      <c r="B12" s="5">
         <v>43707</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -854,12 +885,10 @@
       <c r="K12" s="3"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A13" s="4">
         <v>6</v>
       </c>
-      <c r="B13" s="1">
-        <f t="shared" si="1"/>
+      <c r="B13" s="5">
         <v>43707</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -879,8 +908,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A14" s="4">
         <v>7</v>
       </c>
       <c r="B14" s="5">
@@ -903,12 +931,10 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A15" s="4">
         <v>7</v>
       </c>
-      <c r="B15" s="1">
-        <f t="shared" si="1"/>
+      <c r="B15" s="5">
         <v>43714</v>
       </c>
       <c r="C15" s="4" t="s">
@@ -928,12 +954,10 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A16" s="4">
         <v>8</v>
       </c>
-      <c r="B16" s="1">
-        <f t="shared" si="1"/>
+      <c r="B16" s="5">
         <v>43714</v>
       </c>
       <c r="C16" s="4" t="s">
@@ -953,12 +977,10 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A17" s="4">
         <v>8</v>
       </c>
-      <c r="B17" s="1">
-        <f t="shared" si="1"/>
+      <c r="B17" s="5">
         <v>43714</v>
       </c>
       <c r="C17" s="4" t="s">
@@ -978,12 +1000,10 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A18" s="4">
         <v>9</v>
       </c>
-      <c r="B18" s="1">
-        <f t="shared" si="1"/>
+      <c r="B18" s="5">
         <v>43714</v>
       </c>
       <c r="C18" s="4" t="s">
@@ -1003,12 +1023,10 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A19" s="4">
         <v>9</v>
       </c>
-      <c r="B19" s="1">
-        <f t="shared" si="1"/>
+      <c r="B19" s="5">
         <v>43714</v>
       </c>
       <c r="C19" s="4" t="s">
@@ -1028,12 +1046,10 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A20" s="4">
         <v>10</v>
       </c>
-      <c r="B20" s="1">
-        <f t="shared" si="1"/>
+      <c r="B20" s="5">
         <v>43714</v>
       </c>
       <c r="C20" s="4" t="s">
@@ -1053,12 +1069,10 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A21" s="4">
         <v>10</v>
       </c>
-      <c r="B21" s="1">
-        <f t="shared" si="1"/>
+      <c r="B21" s="5">
         <v>43714</v>
       </c>
       <c r="C21" s="4" t="s">
@@ -1078,12 +1092,10 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A22" s="4">
         <v>11</v>
       </c>
-      <c r="B22" s="1">
-        <f t="shared" si="1"/>
+      <c r="B22" s="5">
         <v>43714</v>
       </c>
       <c r="C22" s="4" t="s">
@@ -1103,12 +1115,10 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A23" s="4">
         <v>11</v>
       </c>
-      <c r="B23" s="1">
-        <f t="shared" si="1"/>
+      <c r="B23" s="5">
         <v>43714</v>
       </c>
       <c r="C23" s="4" t="s">
@@ -1128,12 +1138,10 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A24" s="4">
         <v>12</v>
       </c>
-      <c r="B24" s="1">
-        <f t="shared" si="1"/>
+      <c r="B24" s="5">
         <v>43714</v>
       </c>
       <c r="C24" s="4" t="s">
@@ -1153,12 +1161,10 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A25" s="4">
         <v>12</v>
       </c>
-      <c r="B25" s="1">
-        <f t="shared" si="1"/>
+      <c r="B25" s="5">
         <v>43714</v>
       </c>
       <c r="C25" s="4" t="s">
@@ -1178,12 +1184,10 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A26" s="4">
         <v>13</v>
       </c>
-      <c r="B26" s="1">
-        <f t="shared" si="1"/>
+      <c r="B26" s="5">
         <v>43714</v>
       </c>
       <c r="C26" s="4" t="s">
@@ -1203,12 +1207,10 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A27" s="4">
         <v>13</v>
       </c>
-      <c r="B27" s="1">
-        <f t="shared" si="1"/>
+      <c r="B27" s="5">
         <v>43714</v>
       </c>
       <c r="C27" s="4" t="s">
@@ -1228,12 +1230,10 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A28" s="4">
         <v>14</v>
       </c>
-      <c r="B28" s="1">
-        <f t="shared" si="1"/>
+      <c r="B28" s="5">
         <v>43714</v>
       </c>
       <c r="C28" s="4" t="s">
@@ -1253,12 +1253,10 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A29" s="4">
         <v>14</v>
       </c>
-      <c r="B29" s="1">
-        <f t="shared" si="1"/>
+      <c r="B29" s="5">
         <v>43714</v>
       </c>
       <c r="C29" s="4" t="s">
@@ -1278,12 +1276,10 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A30" s="4">
         <v>15</v>
       </c>
-      <c r="B30" s="1">
-        <f t="shared" si="1"/>
+      <c r="B30" s="5">
         <v>43714</v>
       </c>
       <c r="C30" s="4" t="s">
@@ -1303,12 +1299,10 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A31" s="4">
         <v>15</v>
       </c>
-      <c r="B31" s="1">
-        <f t="shared" si="1"/>
+      <c r="B31" s="5">
         <v>43714</v>
       </c>
       <c r="C31" s="4" t="s">
@@ -1328,12 +1322,10 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A32" s="4">
         <v>16</v>
       </c>
-      <c r="B32" s="1">
-        <f t="shared" si="1"/>
+      <c r="B32" s="5">
         <v>43714</v>
       </c>
       <c r="C32" s="4" t="s">
@@ -1353,12 +1345,10 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A33" s="4">
         <v>16</v>
       </c>
-      <c r="B33" s="1">
-        <f t="shared" si="1"/>
+      <c r="B33" s="5">
         <v>43714</v>
       </c>
       <c r="C33" s="4" t="s">
@@ -1378,12 +1368,10 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A34" s="4">
         <v>17</v>
       </c>
-      <c r="B34" s="1">
-        <f t="shared" si="1"/>
+      <c r="B34" s="5">
         <v>43714</v>
       </c>
       <c r="C34" s="4" t="s">
@@ -1403,12 +1391,10 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A35" s="4">
         <v>17</v>
       </c>
-      <c r="B35" s="1">
-        <f t="shared" si="1"/>
+      <c r="B35" s="5">
         <v>43714</v>
       </c>
       <c r="C35" s="4" t="s">
@@ -1428,12 +1414,10 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A36" s="4">
         <v>18</v>
       </c>
-      <c r="B36" s="1">
-        <f t="shared" si="1"/>
+      <c r="B36" s="5">
         <v>43714</v>
       </c>
       <c r="C36" s="4" t="s">
@@ -1453,12 +1437,10 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A37" s="4">
         <v>18</v>
       </c>
-      <c r="B37" s="1">
-        <f t="shared" si="1"/>
+      <c r="B37" s="5">
         <v>43714</v>
       </c>
       <c r="C37" s="4" t="s">
@@ -1478,8 +1460,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A38" s="4">
         <v>19</v>
       </c>
       <c r="B38" s="5">
@@ -1502,12 +1483,10 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A39" s="4">
         <v>19</v>
       </c>
-      <c r="B39" s="1">
-        <f t="shared" si="1"/>
+      <c r="B39" s="5">
         <v>43721</v>
       </c>
       <c r="C39" s="4" t="s">
@@ -1527,12 +1506,10 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A40" s="4">
         <v>20</v>
       </c>
-      <c r="B40" s="1">
-        <f t="shared" si="1"/>
+      <c r="B40" s="5">
         <v>43721</v>
       </c>
       <c r="C40" s="4" t="s">
@@ -1552,12 +1529,10 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A41" s="4">
         <v>20</v>
       </c>
-      <c r="B41" s="1">
-        <f t="shared" si="1"/>
+      <c r="B41" s="5">
         <v>43721</v>
       </c>
       <c r="C41" s="4" t="s">
@@ -1577,12 +1552,10 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A42" s="4">
         <v>21</v>
       </c>
-      <c r="B42" s="1">
-        <f t="shared" si="1"/>
+      <c r="B42" s="5">
         <v>43721</v>
       </c>
       <c r="C42" s="4" t="s">
@@ -1602,12 +1575,10 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A43" s="4">
         <v>21</v>
       </c>
-      <c r="B43" s="1">
-        <f t="shared" si="1"/>
+      <c r="B43" s="5">
         <v>43721</v>
       </c>
       <c r="C43" s="4" t="s">
@@ -1627,12 +1598,10 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A44" s="4">
         <v>22</v>
       </c>
-      <c r="B44" s="1">
-        <f t="shared" si="1"/>
+      <c r="B44" s="5">
         <v>43721</v>
       </c>
       <c r="C44" s="4" t="s">
@@ -1652,12 +1621,10 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A45" s="4">
         <v>22</v>
       </c>
-      <c r="B45" s="1">
-        <f t="shared" si="1"/>
+      <c r="B45" s="5">
         <v>43721</v>
       </c>
       <c r="C45" s="4" t="s">
@@ -1677,12 +1644,10 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A46" s="4">
         <v>23</v>
       </c>
-      <c r="B46" s="1">
-        <f t="shared" si="1"/>
+      <c r="B46" s="5">
         <v>43721</v>
       </c>
       <c r="C46" s="4" t="s">
@@ -1702,12 +1667,10 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A47" s="4">
         <v>23</v>
       </c>
-      <c r="B47" s="1">
-        <f t="shared" si="1"/>
+      <c r="B47" s="5">
         <v>43721</v>
       </c>
       <c r="C47" s="4" t="s">
@@ -1727,12 +1690,10 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A48" s="4">
         <v>24</v>
       </c>
-      <c r="B48" s="1">
-        <f t="shared" si="1"/>
+      <c r="B48" s="5">
         <v>43721</v>
       </c>
       <c r="C48" s="4" t="s">
@@ -1752,12 +1713,10 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A49" s="4">
         <v>24</v>
       </c>
-      <c r="B49" s="1">
-        <f t="shared" si="1"/>
+      <c r="B49" s="5">
         <v>43721</v>
       </c>
       <c r="C49" s="4" t="s">
@@ -1777,12 +1736,10 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A50" s="4">
         <v>25</v>
       </c>
-      <c r="B50" s="1">
-        <f t="shared" si="1"/>
+      <c r="B50" s="5">
         <v>43721</v>
       </c>
       <c r="C50" s="4" t="s">
@@ -1802,12 +1759,10 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A51" s="4">
         <v>25</v>
       </c>
-      <c r="B51" s="1">
-        <f t="shared" si="1"/>
+      <c r="B51" s="5">
         <v>43721</v>
       </c>
       <c r="C51" s="4" t="s">
@@ -1827,12 +1782,10 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A52" s="4">
         <v>26</v>
       </c>
-      <c r="B52" s="1">
-        <f t="shared" si="1"/>
+      <c r="B52" s="5">
         <v>43721</v>
       </c>
       <c r="C52" s="4" t="s">
@@ -1852,12 +1805,10 @@
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A53" s="4">
         <v>26</v>
       </c>
-      <c r="B53" s="1">
-        <f t="shared" si="1"/>
+      <c r="B53" s="5">
         <v>43721</v>
       </c>
       <c r="C53" s="4" t="s">
@@ -1877,12 +1828,10 @@
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A54" s="4">
         <v>27</v>
       </c>
-      <c r="B54" s="1">
-        <f t="shared" si="1"/>
+      <c r="B54" s="5">
         <v>43721</v>
       </c>
       <c r="C54" s="4" t="s">
@@ -1902,12 +1851,10 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A55" s="4">
         <v>27</v>
       </c>
-      <c r="B55" s="1">
-        <f t="shared" si="1"/>
+      <c r="B55" s="5">
         <v>43721</v>
       </c>
       <c r="C55" s="4" t="s">
@@ -1927,12 +1874,10 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A56" s="4">
         <v>28</v>
       </c>
-      <c r="B56" s="1">
-        <f t="shared" si="1"/>
+      <c r="B56" s="5">
         <v>43721</v>
       </c>
       <c r="C56" s="4" t="s">
@@ -1952,12 +1897,10 @@
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A57" s="4">
         <v>28</v>
       </c>
-      <c r="B57" s="1">
-        <f t="shared" si="1"/>
+      <c r="B57" s="5">
         <v>43721</v>
       </c>
       <c r="C57" s="4" t="s">
@@ -1977,12 +1920,10 @@
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A58" s="4">
         <v>29</v>
       </c>
-      <c r="B58" s="1">
-        <f t="shared" si="1"/>
+      <c r="B58" s="5">
         <v>43721</v>
       </c>
       <c r="C58" s="4" t="s">
@@ -2002,12 +1943,10 @@
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A59" s="4">
         <v>29</v>
       </c>
-      <c r="B59" s="1">
-        <f t="shared" si="1"/>
+      <c r="B59" s="5">
         <v>43721</v>
       </c>
       <c r="C59" s="4" t="s">
@@ -2027,12 +1966,10 @@
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A60" s="4">
         <v>30</v>
       </c>
-      <c r="B60" s="1">
-        <f t="shared" si="1"/>
+      <c r="B60" s="5">
         <v>43721</v>
       </c>
       <c r="C60" s="4" t="s">
@@ -2052,12 +1989,10 @@
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A61" s="4">
         <v>30</v>
       </c>
-      <c r="B61" s="1">
-        <f t="shared" si="1"/>
+      <c r="B61" s="5">
         <v>43721</v>
       </c>
       <c r="C61" s="4" t="s">
@@ -2077,12 +2012,10 @@
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A62" s="4">
         <v>31</v>
       </c>
-      <c r="B62" s="1">
-        <f t="shared" si="1"/>
+      <c r="B62" s="5">
         <v>43721</v>
       </c>
       <c r="C62" s="4" t="s">
@@ -2102,12 +2035,10 @@
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A63" s="4">
         <v>31</v>
       </c>
-      <c r="B63" s="1">
-        <f t="shared" si="1"/>
+      <c r="B63" s="5">
         <v>43721</v>
       </c>
       <c r="C63" s="4" t="s">
@@ -2127,8 +2058,7 @@
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A64" s="4">
         <v>32</v>
       </c>
       <c r="B64" s="5">
@@ -2151,12 +2081,10 @@
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A65" s="4">
         <v>32</v>
       </c>
-      <c r="B65" s="1">
-        <f t="shared" si="1"/>
+      <c r="B65" s="5">
         <v>43728</v>
       </c>
       <c r="C65" s="4" t="s">
@@ -2176,12 +2104,10 @@
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A66" s="4">
         <v>33</v>
       </c>
-      <c r="B66" s="1">
-        <f t="shared" si="1"/>
+      <c r="B66" s="5">
         <v>43728</v>
       </c>
       <c r="C66" s="4" t="s">
@@ -2201,12 +2127,10 @@
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67">
-        <f t="shared" ca="1" si="0"/>
+      <c r="A67" s="4">
         <v>33</v>
       </c>
-      <c r="B67" s="1">
-        <f t="shared" si="1"/>
+      <c r="B67" s="5">
         <v>43728</v>
       </c>
       <c r="C67" s="4" t="s">
@@ -2226,12 +2150,10 @@
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68">
-        <f t="shared" ref="A68:A105" ca="1" si="2">IF(ISEVEN( CELL("row",A68)) = TRUE, A67 + 1, A67)</f>
+      <c r="A68" s="4">
         <v>34</v>
       </c>
-      <c r="B68" s="1">
-        <f t="shared" ref="B68:B83" si="3">B67</f>
+      <c r="B68" s="5">
         <v>43728</v>
       </c>
       <c r="C68" s="4" t="s">
@@ -2251,12 +2173,10 @@
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69">
-        <f t="shared" ca="1" si="2"/>
+      <c r="A69" s="4">
         <v>34</v>
       </c>
-      <c r="B69" s="1">
-        <f t="shared" si="3"/>
+      <c r="B69" s="5">
         <v>43728</v>
       </c>
       <c r="C69" s="4" t="s">
@@ -2276,12 +2196,10 @@
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70">
-        <f t="shared" ca="1" si="2"/>
+      <c r="A70" s="4">
         <v>35</v>
       </c>
-      <c r="B70" s="1">
-        <f t="shared" si="3"/>
+      <c r="B70" s="5">
         <v>43728</v>
       </c>
       <c r="C70" s="4" t="s">
@@ -2301,12 +2219,10 @@
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71">
-        <f t="shared" ca="1" si="2"/>
+      <c r="A71" s="4">
         <v>35</v>
       </c>
-      <c r="B71" s="1">
-        <f t="shared" si="3"/>
+      <c r="B71" s="5">
         <v>43728</v>
       </c>
       <c r="C71" s="4" t="s">
@@ -2326,12 +2242,10 @@
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72">
-        <f t="shared" ca="1" si="2"/>
+      <c r="A72" s="4">
         <v>36</v>
       </c>
-      <c r="B72" s="1">
-        <f t="shared" si="3"/>
+      <c r="B72" s="5">
         <v>43728</v>
       </c>
       <c r="C72" s="4" t="s">
@@ -2351,12 +2265,10 @@
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73">
-        <f t="shared" ca="1" si="2"/>
+      <c r="A73" s="4">
         <v>36</v>
       </c>
-      <c r="B73" s="1">
-        <f t="shared" si="3"/>
+      <c r="B73" s="5">
         <v>43728</v>
       </c>
       <c r="C73" s="4" t="s">
@@ -2376,12 +2288,10 @@
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74">
-        <f t="shared" ca="1" si="2"/>
+      <c r="A74" s="4">
         <v>37</v>
       </c>
-      <c r="B74" s="1">
-        <f t="shared" si="3"/>
+      <c r="B74" s="5">
         <v>43728</v>
       </c>
       <c r="C74" s="4" t="s">
@@ -2401,12 +2311,10 @@
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75">
-        <f t="shared" ca="1" si="2"/>
+      <c r="A75" s="4">
         <v>37</v>
       </c>
-      <c r="B75" s="1">
-        <f t="shared" si="3"/>
+      <c r="B75" s="5">
         <v>43728</v>
       </c>
       <c r="C75" s="4" t="s">
@@ -2426,12 +2334,10 @@
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76">
-        <f t="shared" ca="1" si="2"/>
+      <c r="A76" s="4">
         <v>38</v>
       </c>
-      <c r="B76" s="1">
-        <f t="shared" si="3"/>
+      <c r="B76" s="5">
         <v>43728</v>
       </c>
       <c r="C76" s="4" t="s">
@@ -2451,12 +2357,10 @@
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77">
-        <f t="shared" ca="1" si="2"/>
+      <c r="A77" s="4">
         <v>38</v>
       </c>
-      <c r="B77" s="1">
-        <f t="shared" si="3"/>
+      <c r="B77" s="5">
         <v>43728</v>
       </c>
       <c r="C77" s="4" t="s">
@@ -2476,12 +2380,10 @@
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78">
-        <f t="shared" ca="1" si="2"/>
+      <c r="A78" s="4">
         <v>39</v>
       </c>
-      <c r="B78" s="1">
-        <f t="shared" si="3"/>
+      <c r="B78" s="5">
         <v>43728</v>
       </c>
       <c r="C78" s="4" t="s">
@@ -2501,12 +2403,10 @@
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79">
-        <f t="shared" ca="1" si="2"/>
+      <c r="A79" s="4">
         <v>39</v>
       </c>
-      <c r="B79" s="1">
-        <f t="shared" si="3"/>
+      <c r="B79" s="5">
         <v>43728</v>
       </c>
       <c r="C79" s="4" t="s">
@@ -2526,12 +2426,10 @@
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80">
-        <f t="shared" ca="1" si="2"/>
+      <c r="A80" s="4">
         <v>40</v>
       </c>
-      <c r="B80" s="1">
-        <f t="shared" si="3"/>
+      <c r="B80" s="5">
         <v>43728</v>
       </c>
       <c r="C80" s="4" t="s">
@@ -2551,12 +2449,10 @@
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81">
-        <f t="shared" ca="1" si="2"/>
+      <c r="A81" s="4">
         <v>40</v>
       </c>
-      <c r="B81" s="1">
-        <f t="shared" si="3"/>
+      <c r="B81" s="5">
         <v>43728</v>
       </c>
       <c r="C81" s="4" t="s">
@@ -2576,12 +2472,10 @@
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82">
-        <f t="shared" ca="1" si="2"/>
+      <c r="A82" s="4">
         <v>41</v>
       </c>
-      <c r="B82" s="1">
-        <f t="shared" si="3"/>
+      <c r="B82" s="5">
         <v>43728</v>
       </c>
       <c r="C82" s="4" t="s">
@@ -2601,12 +2495,10 @@
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83">
-        <f t="shared" ca="1" si="2"/>
+      <c r="A83" s="4">
         <v>41</v>
       </c>
-      <c r="B83" s="1">
-        <f t="shared" si="3"/>
+      <c r="B83" s="5">
         <v>43728</v>
       </c>
       <c r="C83" s="4" t="s">
@@ -2626,11 +2518,10 @@
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84">
-        <f t="shared" ca="1" si="2"/>
+      <c r="A84" s="4">
         <v>42</v>
       </c>
-      <c r="B84" s="1">
+      <c r="B84" s="5">
         <v>43734</v>
       </c>
       <c r="C84" s="4" t="s">
@@ -2650,11 +2541,10 @@
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A85">
-        <f t="shared" ca="1" si="2"/>
+      <c r="A85" s="4">
         <v>42</v>
       </c>
-      <c r="B85" s="1">
+      <c r="B85" s="5">
         <v>43734</v>
       </c>
       <c r="C85" s="4" t="s">
@@ -2674,11 +2564,10 @@
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86">
-        <f t="shared" ca="1" si="2"/>
+      <c r="A86" s="4">
         <v>43</v>
       </c>
-      <c r="B86" s="1">
+      <c r="B86" s="5">
         <v>43734</v>
       </c>
       <c r="C86" s="4" t="s">
@@ -2698,11 +2587,10 @@
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87">
-        <f t="shared" ca="1" si="2"/>
+      <c r="A87" s="4">
         <v>43</v>
       </c>
-      <c r="B87" s="1">
+      <c r="B87" s="5">
         <v>43734</v>
       </c>
       <c r="C87" s="4" t="s">
@@ -2722,11 +2610,10 @@
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A88">
-        <f t="shared" ca="1" si="2"/>
+      <c r="A88" s="4">
         <v>44</v>
       </c>
-      <c r="B88" s="1">
+      <c r="B88" s="5">
         <v>43734</v>
       </c>
       <c r="C88" s="4" t="s">
@@ -2746,11 +2633,10 @@
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89">
-        <f t="shared" ca="1" si="2"/>
+      <c r="A89" s="4">
         <v>44</v>
       </c>
-      <c r="B89" s="1">
+      <c r="B89" s="5">
         <v>43734</v>
       </c>
       <c r="C89" s="4" t="s">
@@ -2770,11 +2656,10 @@
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90">
-        <f t="shared" ca="1" si="2"/>
+      <c r="A90" s="4">
         <v>45</v>
       </c>
-      <c r="B90" s="1">
+      <c r="B90" s="5">
         <v>43734</v>
       </c>
       <c r="C90" s="4" t="s">
@@ -2794,11 +2679,10 @@
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91">
-        <f t="shared" ca="1" si="2"/>
+      <c r="A91" s="4">
         <v>45</v>
       </c>
-      <c r="B91" s="1">
+      <c r="B91" s="5">
         <v>43734</v>
       </c>
       <c r="C91" s="4" t="s">
@@ -2818,11 +2702,10 @@
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92">
-        <f t="shared" ca="1" si="2"/>
+      <c r="A92" s="4">
         <v>46</v>
       </c>
-      <c r="B92" s="1">
+      <c r="B92" s="5">
         <v>43734</v>
       </c>
       <c r="C92" s="4" t="s">
@@ -2842,11 +2725,10 @@
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A93">
-        <f t="shared" ca="1" si="2"/>
+      <c r="A93" s="4">
         <v>46</v>
       </c>
-      <c r="B93" s="1">
+      <c r="B93" s="5">
         <v>43734</v>
       </c>
       <c r="C93" s="4" t="s">
@@ -2866,11 +2748,10 @@
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94">
-        <f t="shared" ca="1" si="2"/>
+      <c r="A94" s="4">
         <v>47</v>
       </c>
-      <c r="B94" s="1">
+      <c r="B94" s="5">
         <v>43734</v>
       </c>
       <c r="C94" s="4" t="s">
@@ -2890,11 +2771,10 @@
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95">
-        <f t="shared" ca="1" si="2"/>
+      <c r="A95" s="4">
         <v>47</v>
       </c>
-      <c r="B95" s="1">
+      <c r="B95" s="5">
         <v>43734</v>
       </c>
       <c r="C95" s="4" t="s">
@@ -2914,11 +2794,10 @@
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96">
-        <f t="shared" ca="1" si="2"/>
+      <c r="A96" s="4">
         <v>48</v>
       </c>
-      <c r="B96" s="1">
+      <c r="B96" s="5">
         <v>43734</v>
       </c>
       <c r="C96" s="4" t="s">
@@ -2938,11 +2817,10 @@
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A97">
-        <f t="shared" ca="1" si="2"/>
+      <c r="A97" s="4">
         <v>48</v>
       </c>
-      <c r="B97" s="1">
+      <c r="B97" s="5">
         <v>43734</v>
       </c>
       <c r="C97" s="4" t="s">
@@ -2962,11 +2840,10 @@
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A98">
-        <f t="shared" ca="1" si="2"/>
+      <c r="A98" s="4">
         <v>49</v>
       </c>
-      <c r="B98" s="1">
+      <c r="B98" s="5">
         <v>43734</v>
       </c>
       <c r="C98" s="4" t="s">
@@ -2986,11 +2863,10 @@
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A99">
-        <f t="shared" ca="1" si="2"/>
+      <c r="A99" s="4">
         <v>49</v>
       </c>
-      <c r="B99" s="1">
+      <c r="B99" s="5">
         <v>43734</v>
       </c>
       <c r="C99" s="4" t="s">
@@ -3010,11 +2886,10 @@
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A100">
-        <f t="shared" ca="1" si="2"/>
+      <c r="A100" s="4">
         <v>50</v>
       </c>
-      <c r="B100" s="1">
+      <c r="B100" s="5">
         <v>43734</v>
       </c>
       <c r="C100" s="4" t="s">
@@ -3034,11 +2909,10 @@
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A101">
-        <f t="shared" ca="1" si="2"/>
+      <c r="A101" s="4">
         <v>50</v>
       </c>
-      <c r="B101" s="1">
+      <c r="B101" s="5">
         <v>43734</v>
       </c>
       <c r="C101" s="4" t="s">
@@ -3058,11 +2932,10 @@
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A102">
-        <f t="shared" ca="1" si="2"/>
+      <c r="A102" s="4">
         <v>51</v>
       </c>
-      <c r="B102" s="1">
+      <c r="B102" s="5">
         <v>43734</v>
       </c>
       <c r="C102" s="4" t="s">
@@ -3082,11 +2955,10 @@
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A103">
-        <f t="shared" ca="1" si="2"/>
+      <c r="A103" s="4">
         <v>51</v>
       </c>
-      <c r="B103" s="1">
+      <c r="B103" s="5">
         <v>43734</v>
       </c>
       <c r="C103" s="4" t="s">
@@ -3106,11 +2978,10 @@
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A104">
-        <f t="shared" ca="1" si="2"/>
+      <c r="A104" s="4">
         <v>52</v>
       </c>
-      <c r="B104" s="1">
+      <c r="B104" s="5">
         <v>43734</v>
       </c>
       <c r="C104" s="4" t="s">
@@ -3130,11 +3001,10 @@
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A105">
-        <f t="shared" ca="1" si="2"/>
+      <c r="A105" s="4">
         <v>52</v>
       </c>
-      <c r="B105" s="1">
+      <c r="B105" s="5">
         <v>43734</v>
       </c>
       <c r="C105" s="4" t="s">
@@ -3151,6 +3021,1892 @@
       </c>
       <c r="G105" s="6">
         <v>294</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" s="4">
+        <v>53</v>
+      </c>
+      <c r="B106" s="5">
+        <v>43756</v>
+      </c>
+      <c r="C106" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D106" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E106" s="4">
+        <v>1</v>
+      </c>
+      <c r="F106" s="4">
+        <v>3</v>
+      </c>
+      <c r="G106" s="6">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107" s="4">
+        <v>53</v>
+      </c>
+      <c r="B107" s="5">
+        <v>43756</v>
+      </c>
+      <c r="C107" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D107" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E107" s="4">
+        <v>0</v>
+      </c>
+      <c r="F107" s="4">
+        <v>2</v>
+      </c>
+      <c r="G107" s="6">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A108" s="4">
+        <v>54</v>
+      </c>
+      <c r="B108" s="5">
+        <v>43756</v>
+      </c>
+      <c r="C108" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D108" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E108" s="4">
+        <v>1</v>
+      </c>
+      <c r="F108" s="4">
+        <v>3</v>
+      </c>
+      <c r="G108" s="6">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109" s="4">
+        <v>54</v>
+      </c>
+      <c r="B109" s="5">
+        <v>43756</v>
+      </c>
+      <c r="C109" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D109" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E109" s="4">
+        <v>0</v>
+      </c>
+      <c r="F109" s="4">
+        <v>0</v>
+      </c>
+      <c r="G109" s="6">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110" s="4">
+        <v>55</v>
+      </c>
+      <c r="B110" s="5">
+        <v>43756</v>
+      </c>
+      <c r="C110" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D110" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E110" s="4">
+        <v>1</v>
+      </c>
+      <c r="F110" s="4">
+        <v>3</v>
+      </c>
+      <c r="G110" s="6">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111" s="4">
+        <v>55</v>
+      </c>
+      <c r="B111" s="5">
+        <v>43756</v>
+      </c>
+      <c r="C111" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D111" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E111" s="4">
+        <v>0</v>
+      </c>
+      <c r="F111" s="4">
+        <v>0</v>
+      </c>
+      <c r="G111" s="6">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112" s="4">
+        <v>56</v>
+      </c>
+      <c r="B112" s="5">
+        <v>43756</v>
+      </c>
+      <c r="C112" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D112" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E112" s="4">
+        <v>1</v>
+      </c>
+      <c r="F112" s="4">
+        <v>3</v>
+      </c>
+      <c r="G112" s="6">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A113" s="4">
+        <v>56</v>
+      </c>
+      <c r="B113" s="5">
+        <v>43756</v>
+      </c>
+      <c r="C113" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D113" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E113" s="4">
+        <v>0</v>
+      </c>
+      <c r="F113" s="4">
+        <v>0</v>
+      </c>
+      <c r="G113" s="6">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A114" s="4">
+        <v>57</v>
+      </c>
+      <c r="B114" s="5">
+        <v>43756</v>
+      </c>
+      <c r="C114" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D114" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E114" s="4">
+        <v>0</v>
+      </c>
+      <c r="F114" s="4">
+        <v>1</v>
+      </c>
+      <c r="G114" s="6">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A115" s="4">
+        <v>57</v>
+      </c>
+      <c r="B115" s="5">
+        <v>43756</v>
+      </c>
+      <c r="C115" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D115" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E115" s="4">
+        <v>1</v>
+      </c>
+      <c r="F115" s="4">
+        <v>3</v>
+      </c>
+      <c r="G115" s="6">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A116" s="4">
+        <v>58</v>
+      </c>
+      <c r="B116" s="5">
+        <v>43756</v>
+      </c>
+      <c r="C116" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D116" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E116" s="4">
+        <v>1</v>
+      </c>
+      <c r="F116" s="4">
+        <v>3</v>
+      </c>
+      <c r="G116" s="6">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A117" s="4">
+        <v>58</v>
+      </c>
+      <c r="B117" s="5">
+        <v>43756</v>
+      </c>
+      <c r="C117" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D117" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E117" s="4">
+        <v>0</v>
+      </c>
+      <c r="F117" s="4">
+        <v>0</v>
+      </c>
+      <c r="G117" s="6">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A118" s="4">
+        <v>59</v>
+      </c>
+      <c r="B118" s="5">
+        <v>43756</v>
+      </c>
+      <c r="C118" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D118" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E118" s="4">
+        <v>1</v>
+      </c>
+      <c r="F118" s="4">
+        <v>3</v>
+      </c>
+      <c r="G118" s="6">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A119" s="4">
+        <v>59</v>
+      </c>
+      <c r="B119" s="5">
+        <v>43756</v>
+      </c>
+      <c r="C119" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D119" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E119" s="4">
+        <v>0</v>
+      </c>
+      <c r="F119" s="4">
+        <v>0</v>
+      </c>
+      <c r="G119" s="6">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A120" s="4">
+        <v>60</v>
+      </c>
+      <c r="B120" s="5">
+        <v>43756</v>
+      </c>
+      <c r="C120" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D120" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E120" s="4">
+        <v>0</v>
+      </c>
+      <c r="F120" s="4">
+        <v>0</v>
+      </c>
+      <c r="G120" s="6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A121" s="4">
+        <v>60</v>
+      </c>
+      <c r="B121" s="5">
+        <v>43756</v>
+      </c>
+      <c r="C121" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D121" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E121" s="4">
+        <v>1</v>
+      </c>
+      <c r="F121" s="4">
+        <v>3</v>
+      </c>
+      <c r="G121" s="6">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A122" s="4">
+        <v>61</v>
+      </c>
+      <c r="B122" s="5">
+        <v>43756</v>
+      </c>
+      <c r="C122" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D122" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E122" s="4">
+        <v>1</v>
+      </c>
+      <c r="F122" s="4">
+        <v>3</v>
+      </c>
+      <c r="G122" s="6">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A123" s="4">
+        <v>61</v>
+      </c>
+      <c r="B123" s="5">
+        <v>43756</v>
+      </c>
+      <c r="C123" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D123" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E123" s="4">
+        <v>0</v>
+      </c>
+      <c r="F123" s="4">
+        <v>1</v>
+      </c>
+      <c r="G123" s="6">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A124" s="4">
+        <v>62</v>
+      </c>
+      <c r="B124" s="5">
+        <v>43756</v>
+      </c>
+      <c r="C124" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D124" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E124" s="4">
+        <v>0</v>
+      </c>
+      <c r="F124" s="4">
+        <v>2</v>
+      </c>
+      <c r="G124" s="6">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A125" s="4">
+        <v>62</v>
+      </c>
+      <c r="B125" s="5">
+        <v>43756</v>
+      </c>
+      <c r="C125" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D125" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E125" s="4">
+        <v>1</v>
+      </c>
+      <c r="F125" s="4">
+        <v>3</v>
+      </c>
+      <c r="G125" s="6">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A126" s="4">
+        <v>63</v>
+      </c>
+      <c r="B126" s="5">
+        <v>43756</v>
+      </c>
+      <c r="C126" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D126" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E126" s="4">
+        <v>1</v>
+      </c>
+      <c r="F126" s="4">
+        <v>3</v>
+      </c>
+      <c r="G126" s="6">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A127" s="4">
+        <v>63</v>
+      </c>
+      <c r="B127" s="5">
+        <v>43756</v>
+      </c>
+      <c r="C127" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D127" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E127" s="4">
+        <v>0</v>
+      </c>
+      <c r="F127" s="4">
+        <v>1</v>
+      </c>
+      <c r="G127" s="6">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A128" s="4">
+        <v>64</v>
+      </c>
+      <c r="B128" s="5">
+        <v>43756</v>
+      </c>
+      <c r="C128" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D128" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E128" s="4">
+        <v>0</v>
+      </c>
+      <c r="F128" s="4">
+        <v>2</v>
+      </c>
+      <c r="G128" s="6">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A129" s="4">
+        <v>64</v>
+      </c>
+      <c r="B129" s="5">
+        <v>43756</v>
+      </c>
+      <c r="C129" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D129" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E129" s="4">
+        <v>1</v>
+      </c>
+      <c r="F129" s="4">
+        <v>3</v>
+      </c>
+      <c r="G129" s="6">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A130" s="4">
+        <v>65</v>
+      </c>
+      <c r="B130" s="5">
+        <v>43756</v>
+      </c>
+      <c r="C130" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D130" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E130" s="4">
+        <v>0</v>
+      </c>
+      <c r="F130" s="4">
+        <v>2</v>
+      </c>
+      <c r="G130" s="6">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A131" s="4">
+        <v>65</v>
+      </c>
+      <c r="B131" s="5">
+        <v>43756</v>
+      </c>
+      <c r="C131" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D131" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E131" s="4">
+        <v>1</v>
+      </c>
+      <c r="F131" s="4">
+        <v>3</v>
+      </c>
+      <c r="G131" s="6">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A132" s="4">
+        <v>66</v>
+      </c>
+      <c r="B132" s="5">
+        <v>43756</v>
+      </c>
+      <c r="C132" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D132" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E132" s="4">
+        <v>0</v>
+      </c>
+      <c r="F132" s="4">
+        <v>2</v>
+      </c>
+      <c r="G132" s="6">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A133" s="4">
+        <v>66</v>
+      </c>
+      <c r="B133" s="5">
+        <v>43756</v>
+      </c>
+      <c r="C133" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D133" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E133" s="4">
+        <v>1</v>
+      </c>
+      <c r="F133" s="4">
+        <v>3</v>
+      </c>
+      <c r="G133" s="6">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A134" s="4">
+        <v>67</v>
+      </c>
+      <c r="B134" s="5">
+        <v>43756</v>
+      </c>
+      <c r="C134" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D134" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E134" s="4">
+        <v>1</v>
+      </c>
+      <c r="F134" s="4">
+        <v>3</v>
+      </c>
+      <c r="G134" s="6">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A135" s="4">
+        <v>67</v>
+      </c>
+      <c r="B135" s="5">
+        <v>43756</v>
+      </c>
+      <c r="C135" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D135" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E135" s="4">
+        <v>0</v>
+      </c>
+      <c r="F135" s="4">
+        <v>1</v>
+      </c>
+      <c r="G135" s="6">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A136" s="4">
+        <v>68</v>
+      </c>
+      <c r="B136" s="5">
+        <v>43756</v>
+      </c>
+      <c r="C136" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D136" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E136" s="4">
+        <v>0</v>
+      </c>
+      <c r="F136" s="4">
+        <v>2</v>
+      </c>
+      <c r="G136" s="6">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A137" s="4">
+        <v>68</v>
+      </c>
+      <c r="B137" s="5">
+        <v>43756</v>
+      </c>
+      <c r="C137" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D137" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E137" s="4">
+        <v>1</v>
+      </c>
+      <c r="F137" s="4">
+        <v>3</v>
+      </c>
+      <c r="G137" s="6">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A138" s="4">
+        <v>69</v>
+      </c>
+      <c r="B138" s="5">
+        <v>43756</v>
+      </c>
+      <c r="C138" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D138" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E138" s="4">
+        <v>1</v>
+      </c>
+      <c r="F138" s="4">
+        <v>3</v>
+      </c>
+      <c r="G138" s="6">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A139" s="4">
+        <v>69</v>
+      </c>
+      <c r="B139" s="5">
+        <v>43756</v>
+      </c>
+      <c r="C139" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D139" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E139" s="4">
+        <v>0</v>
+      </c>
+      <c r="F139" s="4">
+        <v>1</v>
+      </c>
+      <c r="G139" s="6">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A140" s="4">
+        <v>70</v>
+      </c>
+      <c r="B140" s="5">
+        <v>43756</v>
+      </c>
+      <c r="C140" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D140" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E140" s="4">
+        <v>1</v>
+      </c>
+      <c r="F140" s="4">
+        <v>3</v>
+      </c>
+      <c r="G140" s="6">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A141" s="4">
+        <v>70</v>
+      </c>
+      <c r="B141" s="5">
+        <v>43756</v>
+      </c>
+      <c r="C141" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D141" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E141" s="4">
+        <v>0</v>
+      </c>
+      <c r="F141" s="4">
+        <v>2</v>
+      </c>
+      <c r="G141" s="6">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A142" s="4">
+        <v>71</v>
+      </c>
+      <c r="B142" s="5">
+        <v>43763</v>
+      </c>
+      <c r="C142" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D142" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E142" s="4">
+        <v>0</v>
+      </c>
+      <c r="F142" s="4">
+        <v>2</v>
+      </c>
+      <c r="G142" s="6">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A143" s="4">
+        <v>71</v>
+      </c>
+      <c r="B143" s="5">
+        <v>43763</v>
+      </c>
+      <c r="C143" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D143" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E143" s="4">
+        <v>1</v>
+      </c>
+      <c r="F143" s="4">
+        <v>3</v>
+      </c>
+      <c r="G143" s="6">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A144" s="4">
+        <v>72</v>
+      </c>
+      <c r="B144" s="5">
+        <v>43763</v>
+      </c>
+      <c r="C144" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D144" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E144" s="4">
+        <v>1</v>
+      </c>
+      <c r="F144" s="4">
+        <v>3</v>
+      </c>
+      <c r="G144" s="6">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A145" s="4">
+        <v>72</v>
+      </c>
+      <c r="B145" s="5">
+        <v>43763</v>
+      </c>
+      <c r="C145" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D145" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E145" s="4">
+        <v>0</v>
+      </c>
+      <c r="F145" s="4">
+        <v>1</v>
+      </c>
+      <c r="G145" s="6">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A146" s="4">
+        <v>73</v>
+      </c>
+      <c r="B146" s="5">
+        <v>43763</v>
+      </c>
+      <c r="C146" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D146" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E146" s="4">
+        <v>0</v>
+      </c>
+      <c r="F146" s="4">
+        <v>1</v>
+      </c>
+      <c r="G146" s="6">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A147" s="4">
+        <v>73</v>
+      </c>
+      <c r="B147" s="5">
+        <v>43763</v>
+      </c>
+      <c r="C147" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D147" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E147" s="4">
+        <v>1</v>
+      </c>
+      <c r="F147" s="4">
+        <v>3</v>
+      </c>
+      <c r="G147" s="6">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A148" s="4">
+        <v>74</v>
+      </c>
+      <c r="B148" s="5">
+        <v>43763</v>
+      </c>
+      <c r="C148" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D148" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E148" s="4">
+        <v>1</v>
+      </c>
+      <c r="F148" s="4">
+        <v>3</v>
+      </c>
+      <c r="G148" s="6">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A149" s="4">
+        <v>74</v>
+      </c>
+      <c r="B149" s="5">
+        <v>43763</v>
+      </c>
+      <c r="C149" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D149" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E149" s="4">
+        <v>0</v>
+      </c>
+      <c r="F149" s="4">
+        <v>1</v>
+      </c>
+      <c r="G149" s="6">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A150" s="4">
+        <v>75</v>
+      </c>
+      <c r="B150" s="5">
+        <v>43763</v>
+      </c>
+      <c r="C150" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D150" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E150" s="4">
+        <v>1</v>
+      </c>
+      <c r="F150" s="4">
+        <v>3</v>
+      </c>
+      <c r="G150" s="6">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A151" s="4">
+        <v>75</v>
+      </c>
+      <c r="B151" s="5">
+        <v>43763</v>
+      </c>
+      <c r="C151" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D151" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E151" s="4">
+        <v>0</v>
+      </c>
+      <c r="F151" s="4">
+        <v>2</v>
+      </c>
+      <c r="G151" s="6">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A152" s="4">
+        <v>76</v>
+      </c>
+      <c r="B152" s="5">
+        <v>43763</v>
+      </c>
+      <c r="C152" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D152" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E152" s="4">
+        <v>1</v>
+      </c>
+      <c r="F152" s="4">
+        <v>3</v>
+      </c>
+      <c r="G152" s="6">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A153" s="4">
+        <v>76</v>
+      </c>
+      <c r="B153" s="5">
+        <v>43763</v>
+      </c>
+      <c r="C153" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D153" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E153" s="4">
+        <v>0</v>
+      </c>
+      <c r="F153" s="4">
+        <v>1</v>
+      </c>
+      <c r="G153" s="6">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A154" s="4">
+        <v>77</v>
+      </c>
+      <c r="B154" s="5">
+        <v>43763</v>
+      </c>
+      <c r="C154" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D154" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E154" s="4">
+        <v>1</v>
+      </c>
+      <c r="F154" s="4">
+        <v>3</v>
+      </c>
+      <c r="G154" s="6">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A155" s="4">
+        <v>77</v>
+      </c>
+      <c r="B155" s="5">
+        <v>43763</v>
+      </c>
+      <c r="C155" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D155" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E155" s="4">
+        <v>0</v>
+      </c>
+      <c r="F155" s="4">
+        <v>2</v>
+      </c>
+      <c r="G155" s="6">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A156" s="4">
+        <v>78</v>
+      </c>
+      <c r="B156" s="5">
+        <v>43763</v>
+      </c>
+      <c r="C156" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D156" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E156" s="4">
+        <v>0</v>
+      </c>
+      <c r="F156" s="4">
+        <v>2</v>
+      </c>
+      <c r="G156" s="6">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A157" s="4">
+        <v>78</v>
+      </c>
+      <c r="B157" s="5">
+        <v>43763</v>
+      </c>
+      <c r="C157" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D157" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E157" s="4">
+        <v>1</v>
+      </c>
+      <c r="F157" s="4">
+        <v>3</v>
+      </c>
+      <c r="G157" s="6">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A158" s="4">
+        <v>79</v>
+      </c>
+      <c r="B158" s="5">
+        <v>43763</v>
+      </c>
+      <c r="C158" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D158" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E158" s="4">
+        <v>1</v>
+      </c>
+      <c r="F158" s="4">
+        <v>3</v>
+      </c>
+      <c r="G158" s="6">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A159" s="4">
+        <v>79</v>
+      </c>
+      <c r="B159" s="5">
+        <v>43763</v>
+      </c>
+      <c r="C159" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D159" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E159" s="4">
+        <v>0</v>
+      </c>
+      <c r="F159" s="4">
+        <v>1</v>
+      </c>
+      <c r="G159" s="6">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A160" s="4">
+        <v>80</v>
+      </c>
+      <c r="B160" s="5">
+        <v>43763</v>
+      </c>
+      <c r="C160" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D160" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E160" s="4">
+        <v>0</v>
+      </c>
+      <c r="F160" s="4">
+        <v>2</v>
+      </c>
+      <c r="G160" s="6">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A161" s="4">
+        <v>80</v>
+      </c>
+      <c r="B161" s="5">
+        <v>43763</v>
+      </c>
+      <c r="C161" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D161" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E161" s="4">
+        <v>1</v>
+      </c>
+      <c r="F161" s="4">
+        <v>3</v>
+      </c>
+      <c r="G161" s="6">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A162" s="4">
+        <v>81</v>
+      </c>
+      <c r="B162" s="5">
+        <v>43763</v>
+      </c>
+      <c r="C162" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D162" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E162" s="4">
+        <v>0</v>
+      </c>
+      <c r="F162" s="4">
+        <v>2</v>
+      </c>
+      <c r="G162" s="6">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A163" s="4">
+        <v>81</v>
+      </c>
+      <c r="B163" s="5">
+        <v>43763</v>
+      </c>
+      <c r="C163" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D163" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E163" s="4">
+        <v>1</v>
+      </c>
+      <c r="F163" s="4">
+        <v>3</v>
+      </c>
+      <c r="G163" s="6">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A164" s="4">
+        <v>82</v>
+      </c>
+      <c r="B164" s="5">
+        <v>43763</v>
+      </c>
+      <c r="C164" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D164" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E164" s="4">
+        <v>1</v>
+      </c>
+      <c r="F164" s="4">
+        <v>3</v>
+      </c>
+      <c r="G164" s="6">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A165" s="4">
+        <v>82</v>
+      </c>
+      <c r="B165" s="5">
+        <v>43763</v>
+      </c>
+      <c r="C165" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D165" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E165" s="4">
+        <v>0</v>
+      </c>
+      <c r="F165" s="4">
+        <v>2</v>
+      </c>
+      <c r="G165" s="6">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A166" s="4">
+        <v>83</v>
+      </c>
+      <c r="B166" s="5">
+        <v>43763</v>
+      </c>
+      <c r="C166" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D166" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E166" s="4">
+        <v>0</v>
+      </c>
+      <c r="F166" s="4">
+        <v>1</v>
+      </c>
+      <c r="G166" s="6">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A167" s="4">
+        <v>83</v>
+      </c>
+      <c r="B167" s="5">
+        <v>43763</v>
+      </c>
+      <c r="C167" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D167" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E167" s="4">
+        <v>1</v>
+      </c>
+      <c r="F167" s="4">
+        <v>3</v>
+      </c>
+      <c r="G167" s="6">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A168" s="4">
+        <v>84</v>
+      </c>
+      <c r="B168" s="5">
+        <v>43763</v>
+      </c>
+      <c r="C168" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D168" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E168" s="4">
+        <v>1</v>
+      </c>
+      <c r="F168" s="4">
+        <v>3</v>
+      </c>
+      <c r="G168" s="6">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A169" s="4">
+        <v>84</v>
+      </c>
+      <c r="B169" s="5">
+        <v>43763</v>
+      </c>
+      <c r="C169" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D169" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E169" s="4">
+        <v>0</v>
+      </c>
+      <c r="F169" s="4">
+        <v>2</v>
+      </c>
+      <c r="G169" s="6">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A170" s="4">
+        <v>85</v>
+      </c>
+      <c r="B170" s="5">
+        <v>43763</v>
+      </c>
+      <c r="C170" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D170" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E170" s="4">
+        <v>1</v>
+      </c>
+      <c r="F170" s="4">
+        <v>3</v>
+      </c>
+      <c r="G170" s="6">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A171" s="4">
+        <v>85</v>
+      </c>
+      <c r="B171" s="5">
+        <v>43763</v>
+      </c>
+      <c r="C171" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D171" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E171" s="4">
+        <v>0</v>
+      </c>
+      <c r="F171" s="4">
+        <v>1</v>
+      </c>
+      <c r="G171" s="6">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A172" s="4">
+        <v>86</v>
+      </c>
+      <c r="B172" s="5">
+        <v>43763</v>
+      </c>
+      <c r="C172" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D172" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E172" s="4">
+        <v>1</v>
+      </c>
+      <c r="F172" s="4">
+        <v>3</v>
+      </c>
+      <c r="G172" s="6">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A173" s="4">
+        <v>86</v>
+      </c>
+      <c r="B173" s="5">
+        <v>43763</v>
+      </c>
+      <c r="C173" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D173" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E173" s="4">
+        <v>0</v>
+      </c>
+      <c r="F173" s="4">
+        <v>2</v>
+      </c>
+      <c r="G173" s="6">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A174" s="4">
+        <v>87</v>
+      </c>
+      <c r="B174" s="5">
+        <v>43763</v>
+      </c>
+      <c r="C174" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D174" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E174" s="4">
+        <v>0</v>
+      </c>
+      <c r="F174" s="4">
+        <v>2</v>
+      </c>
+      <c r="G174" s="6">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A175" s="4">
+        <v>87</v>
+      </c>
+      <c r="B175" s="5">
+        <v>43763</v>
+      </c>
+      <c r="C175" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D175" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E175" s="4">
+        <v>1</v>
+      </c>
+      <c r="F175" s="4">
+        <v>3</v>
+      </c>
+      <c r="G175" s="6">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A176" s="4">
+        <v>88</v>
+      </c>
+      <c r="B176" s="5">
+        <v>43763</v>
+      </c>
+      <c r="C176" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D176" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E176" s="4">
+        <v>0</v>
+      </c>
+      <c r="F176" s="4">
+        <v>1</v>
+      </c>
+      <c r="G176" s="6">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A177" s="4">
+        <v>88</v>
+      </c>
+      <c r="B177" s="5">
+        <v>43763</v>
+      </c>
+      <c r="C177" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D177" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E177" s="4">
+        <v>1</v>
+      </c>
+      <c r="F177" s="4">
+        <v>3</v>
+      </c>
+      <c r="G177" s="6">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A178" s="4">
+        <v>89</v>
+      </c>
+      <c r="B178" s="5">
+        <v>43763</v>
+      </c>
+      <c r="C178" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D178" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E178" s="4">
+        <v>0</v>
+      </c>
+      <c r="F178" s="4">
+        <v>1</v>
+      </c>
+      <c r="G178" s="6">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A179" s="4">
+        <v>89</v>
+      </c>
+      <c r="B179" s="5">
+        <v>43763</v>
+      </c>
+      <c r="C179" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D179" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E179" s="4">
+        <v>1</v>
+      </c>
+      <c r="F179" s="4">
+        <v>3</v>
+      </c>
+      <c r="G179" s="6">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A180" s="4">
+        <v>90</v>
+      </c>
+      <c r="B180" s="5">
+        <v>43763</v>
+      </c>
+      <c r="C180" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D180" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E180" s="4">
+        <v>0</v>
+      </c>
+      <c r="F180" s="4">
+        <v>2</v>
+      </c>
+      <c r="G180" s="6">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A181" s="4">
+        <v>90</v>
+      </c>
+      <c r="B181" s="5">
+        <v>43763</v>
+      </c>
+      <c r="C181" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D181" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E181" s="4">
+        <v>1</v>
+      </c>
+      <c r="F181" s="4">
+        <v>3</v>
+      </c>
+      <c r="G181" s="6">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A182" s="4">
+        <v>91</v>
+      </c>
+      <c r="B182" s="5">
+        <v>43763</v>
+      </c>
+      <c r="C182" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D182" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E182" s="4">
+        <v>0</v>
+      </c>
+      <c r="F182" s="4">
+        <v>1</v>
+      </c>
+      <c r="G182" s="6">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A183" s="4">
+        <v>91</v>
+      </c>
+      <c r="B183" s="5">
+        <v>43763</v>
+      </c>
+      <c r="C183" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D183" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E183" s="4">
+        <v>1</v>
+      </c>
+      <c r="F183" s="4">
+        <v>3</v>
+      </c>
+      <c r="G183" s="6">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A184" s="4">
+        <v>92</v>
+      </c>
+      <c r="B184" s="5">
+        <v>43763</v>
+      </c>
+      <c r="C184" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D184" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E184" s="4">
+        <v>0</v>
+      </c>
+      <c r="F184" s="4">
+        <v>0</v>
+      </c>
+      <c r="G184" s="6">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A185" s="4">
+        <v>92</v>
+      </c>
+      <c r="B185" s="5">
+        <v>43763</v>
+      </c>
+      <c r="C185" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D185" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E185" s="4">
+        <v>1</v>
+      </c>
+      <c r="F185" s="4">
+        <v>3</v>
+      </c>
+      <c r="G185" s="6">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A186" s="4">
+        <v>93</v>
+      </c>
+      <c r="B186" s="5">
+        <v>43763</v>
+      </c>
+      <c r="C186" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D186" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E186" s="4">
+        <v>0</v>
+      </c>
+      <c r="F186" s="4">
+        <v>1</v>
+      </c>
+      <c r="G186" s="6">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A187" s="4">
+        <v>93</v>
+      </c>
+      <c r="B187" s="5">
+        <v>43763</v>
+      </c>
+      <c r="C187" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D187" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E187" s="4">
+        <v>1</v>
+      </c>
+      <c r="F187" s="4">
+        <v>3</v>
+      </c>
+      <c r="G187" s="6">
+        <v>310</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed a few data issues around wins
</commit_message>
<xml_diff>
--- a/SSBU Code.xlsx
+++ b/SSBU Code.xlsx
@@ -41,12 +41,6 @@
     <t>Player</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Win</t>
-  </si>
-  <si>
     <t>KO</t>
   </si>
   <si>
@@ -65,9 +59,6 @@
     <t>Fox</t>
   </si>
   <si>
-    <t>Game</t>
-  </si>
-  <si>
     <t>Chris</t>
   </si>
   <si>
@@ -96,6 +87,15 @@
   </si>
   <si>
     <t>Shulk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Game </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Win </t>
   </si>
 </sst>
 </file>
@@ -443,7 +443,7 @@
   <dimension ref="A1:K187"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection sqref="A1:G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,10 +526,10 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>4</v>
@@ -538,13 +538,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -560,13 +560,13 @@
         <v>2</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E2" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G2" s="6">
         <v>203</v>
@@ -584,13 +584,13 @@
         <v>1</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E3" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G3" s="6">
         <v>392</v>
@@ -608,7 +608,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E4" s="4">
         <v>1</v>
@@ -629,10 +629,10 @@
         <v>43805</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>18</v>
       </c>
       <c r="E5" s="4">
         <v>0</v>
@@ -656,7 +656,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E6" s="4">
         <v>1</v>
@@ -677,10 +677,10 @@
         <v>43805</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>18</v>
       </c>
       <c r="E7" s="4">
         <v>0</v>
@@ -704,7 +704,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E8" s="4">
         <v>1</v>
@@ -728,7 +728,7 @@
         <v>0</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E9" s="4">
         <v>0</v>
@@ -752,7 +752,7 @@
         <v>2</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E10" s="4">
         <v>1</v>
@@ -773,10 +773,10 @@
         <v>43805</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E11" s="4">
         <v>0</v>
@@ -800,7 +800,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E12" s="4">
         <v>1</v>
@@ -821,10 +821,10 @@
         <v>43805</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E13" s="4">
         <v>0</v>
@@ -847,7 +847,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E14" s="4">
         <v>1</v>
@@ -867,10 +867,10 @@
         <v>43805</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E15" s="4">
         <v>0</v>
@@ -893,7 +893,7 @@
         <v>2</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E16" s="4">
         <v>0</v>
@@ -916,7 +916,7 @@
         <v>0</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E17" s="4">
         <v>1</v>
@@ -936,10 +936,10 @@
         <v>43805</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E18" s="4">
         <v>0</v>
@@ -959,10 +959,10 @@
         <v>43805</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E19" s="4">
         <v>1</v>
@@ -985,7 +985,7 @@
         <v>0</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E20" s="4">
         <v>1</v>
@@ -1008,7 +1008,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E21" s="4">
         <v>0</v>
@@ -1031,7 +1031,7 @@
         <v>2</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E22" s="4">
         <v>0</v>
@@ -1051,10 +1051,10 @@
         <v>43805</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E23" s="4">
         <v>1</v>
@@ -1077,10 +1077,10 @@
         <v>0</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E24" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F24" s="4">
         <v>3</v>
@@ -1097,13 +1097,13 @@
         <v>43805</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E25" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F25" s="4">
         <v>1</v>
@@ -1123,7 +1123,7 @@
         <v>1</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E26" s="4">
         <v>1</v>
@@ -1143,10 +1143,10 @@
         <v>43805</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E27" s="4">
         <v>0</v>
@@ -1169,7 +1169,7 @@
         <v>1</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E28" s="4">
         <v>1</v>
@@ -1189,10 +1189,10 @@
         <v>43805</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E29" s="4">
         <v>0</v>
@@ -1215,7 +1215,7 @@
         <v>0</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E30" s="4">
         <v>1</v>
@@ -1238,7 +1238,7 @@
         <v>2</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E31" s="4">
         <v>0</v>
@@ -1258,10 +1258,10 @@
         <v>43805</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E32" s="4">
         <v>1</v>
@@ -1281,10 +1281,10 @@
         <v>43805</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E33" s="4">
         <v>0</v>
@@ -1307,7 +1307,7 @@
         <v>0</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E34" s="4">
         <v>1</v>
@@ -1330,7 +1330,7 @@
         <v>1</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E35" s="4">
         <v>0</v>
@@ -1353,7 +1353,7 @@
         <v>2</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E36" s="4">
         <v>1</v>
@@ -1373,10 +1373,10 @@
         <v>43805</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E37" s="4">
         <v>0</v>
@@ -1399,7 +1399,7 @@
         <v>0</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E38" s="4">
         <v>1</v>
@@ -1419,10 +1419,10 @@
         <v>43805</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E39" s="4">
         <v>0</v>
@@ -1445,7 +1445,7 @@
         <v>1</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E40" s="4">
         <v>1</v>
@@ -1468,7 +1468,7 @@
         <v>2</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E41" s="4">
         <v>0</v>
@@ -1491,7 +1491,7 @@
         <v>0</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E42" s="4">
         <v>1</v>
@@ -1511,10 +1511,10 @@
         <v>43805</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E43" s="4">
         <v>0</v>
@@ -1537,7 +1537,7 @@
         <v>2</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E44" s="4">
         <v>1</v>
@@ -1557,10 +1557,10 @@
         <v>43805</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E45" s="4">
         <v>0</v>
@@ -1583,7 +1583,7 @@
         <v>2</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E46" s="4">
         <v>1</v>
@@ -1603,10 +1603,10 @@
         <v>43805</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E47" s="4">
         <v>0</v>
@@ -1629,7 +1629,7 @@
         <v>0</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E48" s="4">
         <v>1</v>
@@ -1652,7 +1652,7 @@
         <v>1</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E49" s="4">
         <v>0</v>

</xml_diff>